<commit_message>
updated mseasles models and results
</commit_message>
<xml_diff>
--- a/Somalia-COVID-impact/Inputs_Baseline_Measles_National.xlsx
+++ b/Somalia-COVID-impact/Inputs_Baseline_Measles_National.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9D76D8-C1FB-E644-8510-2AC15F44136B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66AC097-FEE8-0E40-9019-086575258B76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27880" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27880" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="National" sheetId="2" r:id="rId1"/>
@@ -14,6 +14,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -449,20 +458,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -470,227 +479,193 @@
         <v>0</v>
       </c>
       <c r="C1" s="1">
-        <v>100</v>
-      </c>
-      <c r="D1" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <f>1/14</f>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="D7" s="2">
-        <f>1/14</f>
-        <v>7.1428571428571425E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>0.9</v>
       </c>
-      <c r="D8" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <f>0.32 * 0.85</f>
         <v>0.27200000000000002</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <f>0.005 * 0.85</f>
         <v>4.2500000000000003E-3</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <f>0 * 0.85</f>
         <v>0</v>
       </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <f>0.32 * 0.15</f>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <f>0.005 * 0.15</f>
         <v>7.5000000000000002E-4</v>
       </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <f>0 * 0.15</f>
         <v>0</v>
       </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <f>0.67 * 0.15</f>
         <v>0.10050000000000001</v>
       </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <f>0.67 * 0.85</f>
         <v>0.56950000000000001</v>
       </c>
-      <c r="D17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>